<commit_message>
Auto update crawl results
</commit_message>
<xml_diff>
--- a/result_files/crawl_result.xlsx
+++ b/result_files/crawl_result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,6 +509,204 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025년 전교생 대상 온라인 SW교육 신청 안내 (유료교육 전액 지원)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>관리자</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://swknu.kongju.ac.kr/community/noticedetail.do?seq=38</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025년 SW중심대학 주관학과 사업설명회 자료 공유</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>관리자</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-03-14</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://swknu.kongju.ac.kr/community/noticedetail.do?seq=37</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025년도 한국통신학회 동계종합학술발표회 아이디어 경진대회 참가자 SW마일리지 부여</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>관리자</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-03-14</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://swknu.kongju.ac.kr/community/noticedetail.do?seq=36</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025 국민대학교 코딩역량인증제 인증시험 참가자 SW마일리지 부여</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>관리자</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-03-13</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://swknu.kongju.ac.kr/community/noticedetail.do?seq=35</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ICCAS 2025 해외교육 프로그램 참가 신청 안내(25.08.25-8.31, 오스트리아/해외교육비 지원)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>관리자</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-03-07</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://swknu.kongju.ac.kr/community/noticedetail.do?seq=34</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025년 SW중심대학 주관학과 사업설명회 안내(25.03.13(목) 12시~)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>관리자</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-03-07</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://swknu.kongju.ac.kr/community/noticedetail.do?seq=33</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>[IITP홍보] 2025 미국 CMU AI 심화교육프로그램 파견 교육생 모집 안내(대학원생-국비 교육비 체제비 지원)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>관리자</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-02-10</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://swknu.kongju.ac.kr/community/noticedetail.do?seq=32</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>[소중협] (홍보) 그렙 「2025 프로그래머스 코드챌린지」 개최 안내</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>관리자</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-01-24</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://swknu.kongju.ac.kr/community/noticedetail.do?seq=31</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025년도 SW마에스트로 과정 제16기 연수생 모집 공고 (우수학생 추천)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>관리자</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2025-01-14</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://swknu.kongju.ac.kr/community/noticedetail.do?seq=30</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>